<commit_message>
update file import ycdc
</commit_message>
<xml_diff>
--- a/addons/custom/forlife_stock/static/src/xlsx/template_import_ycdc.xlsx
+++ b/addons/custom/forlife_stock/static/src/xlsx/template_import_ycdc.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Project\m_onnet_odoo_mfl2201er\addons\custom\forlife_stock\static\src\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FORLIFE\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB1C202-EFC6-4184-83ED-A74BA6EAC840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F55FE1C8-2343-4B9A-A218-4C3EB97A38AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{568D4FBB-6B03-477C-9ADA-02213CA4C781}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
-  <si>
-    <t>Cái</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t>03TL3405763</t>
   </si>
@@ -91,7 +88,22 @@
   </si>
   <si>
     <r>
-      <t>Chi tiết / Đơn vị</t>
+      <t xml:space="preserve">Chi tiết / Từ kho </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>(*)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Chi tiết / Đến kho</t>
     </r>
     <r>
       <rPr>
@@ -105,36 +117,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Chi tiết / Từ kho </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>(*)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Chi tiết / Đến kho</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (*)</t>
-    </r>
-  </si>
-  <si>
     <t>Chi tiết / Từ LSX</t>
   </si>
   <si>
@@ -146,7 +128,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-1010000]d/m/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -245,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -258,22 +240,19 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -587,149 +566,133 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D86403F5-7C39-4400-9B6F-B5C944ECB092}">
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="27.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.77734375" customWidth="1"/>
-    <col min="6" max="6" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.21875" customWidth="1"/>
-    <col min="8" max="8" width="21.109375" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="9">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
         <v>45146.708333333336</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="4">
         <v>10</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="6">
+      <c r="D2" s="5">
         <v>888</v>
       </c>
-      <c r="F2" s="6">
+      <c r="E2" s="5">
         <v>999</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="F2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
       <c r="B3" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="4">
         <v>10</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="5">
+        <v>888</v>
+      </c>
+      <c r="E3" s="5">
+        <v>999</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>45178.708333333336</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>0</v>
-      </c>
-      <c r="E3" s="6">
-        <v>888</v>
-      </c>
-      <c r="F3" s="6">
-        <v>999</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="9">
-        <v>45178.708333333336</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>1</v>
       </c>
       <c r="C4" s="4">
         <v>20</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6">
+      <c r="D4" s="5">
         <v>888</v>
       </c>
-      <c r="F4" s="6">
+      <c r="E4" s="5">
         <v>999</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="F4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="10"/>
-      <c r="B5" s="3" t="s">
-        <v>5</v>
       </c>
       <c r="C5" s="4">
         <v>25</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6">
+      <c r="D5" s="5">
         <v>888</v>
       </c>
-      <c r="F5" s="6">
+      <c r="E5" s="5">
         <v>999</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="F5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>3</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trên PR có thông tin kho nhận
trên PR có thông tin kho nhận
</commit_message>
<xml_diff>
--- a/addons/custom/forlife_stock/static/src/xlsx/template_import_ycdc.xlsx
+++ b/addons/custom/forlife_stock/static/src/xlsx/template_import_ycdc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FORLIFE\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Forlife\code\m_onnet_odoo_mfl2201er\addons\custom\forlife_stock\static\src\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F55FE1C8-2343-4B9A-A218-4C3EB97A38AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCBFC4A0-EBE7-4D84-90E2-E06653BE0DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,8 +24,186 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>admin</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{98233237-535F-482B-8090-2CA014EE832E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Điền thông tin mã LSX khi điều chuyển NPL sang nhà gia công/xưởng SX</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{1852B883-DAF3-44B5-BC37-2D6E646C759A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Điền thông tin đơn mua hàng trong trường hợp điều chuyển hàng theo PO</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{EA82F636-8471-4002-82B4-38EE6B78A2DA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Điền mã Barcode của sản phẩm</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{EFBD89FA-D182-425B-9146-8090504DF28B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Chọn kho theo danh sách kho có trên hệ thống</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{F2C56CE1-C679-4FEC-B608-C9A4C6107C18}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Chọn kho theo danh sách kho có trên hệ thống</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{EF52D4C6-F1C7-4D6A-B003-B8FEE31438B8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Chọn mã lệnh sản xuất đã được khai báo trên hệ thống (Trường hợp chuyển lệnh sản xuất)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{AA1BF037-29E0-4134-9585-E001370120B0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Chọn mã lệnh sản xuất đã được khai báo trên hệ thống (Trường hợp điều chuyển cho sản xuất)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>03TL3405763</t>
   </si>
@@ -122,6 +300,24 @@
   <si>
     <t>Chi tiết / Đến LSX</t>
   </si>
+  <si>
+    <t>Lệnh sản xuất</t>
+  </si>
+  <si>
+    <t>Đơn mua hàng</t>
+  </si>
+  <si>
+    <t>Ghi chú</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Điều chuyển cho LSX</t>
+  </si>
+  <si>
+    <t>Điều chuyển cho cửa hàng</t>
+  </si>
 </sst>
 </file>
 
@@ -130,7 +326,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,6 +360,19 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -227,7 +436,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -253,6 +462,12 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,11 +781,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,119 +799,147 @@
     <col min="7" max="7" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>45146.708333333336</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4">
+      <c r="F2" s="4">
         <v>10</v>
       </c>
-      <c r="D2" s="5">
+      <c r="G2" s="5">
         <v>888</v>
       </c>
-      <c r="E2" s="5">
+      <c r="H2" s="5">
         <v>999</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4">
+      <c r="F3" s="4">
         <v>10</v>
       </c>
-      <c r="D3" s="5">
+      <c r="G3" s="5">
         <v>888</v>
       </c>
-      <c r="E3" s="5">
+      <c r="H3" s="5">
         <v>999</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>45178.708333333336</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="4">
+      <c r="F4" s="4">
         <v>20</v>
       </c>
-      <c r="D4" s="5">
+      <c r="G4" s="5">
         <v>888</v>
       </c>
-      <c r="E4" s="5">
+      <c r="H4" s="5">
         <v>999</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="J4" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="4">
+      <c r="F5" s="4">
         <v>25</v>
       </c>
-      <c r="D5" s="5">
+      <c r="G5" s="5">
         <v>888</v>
       </c>
-      <c r="E5" s="5">
+      <c r="H5" s="5">
         <v>999</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="J5" s="5" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>